<commit_message>
login por stalin controlador y html validado
</commit_message>
<xml_diff>
--- a/Pruebas_GUI/planificacion.xlsx
+++ b/Pruebas_GUI/planificacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documentos\2015-B\Apps Libres\proyecto final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stand\Documents\GitHub\App_Libres_Prueba_GUI\Pruebas_GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -549,14 +549,14 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59" customWidth="1"/>
+    <col min="3" max="3" width="86" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
@@ -620,6 +620,9 @@
       <c r="D3" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="E3">
+        <v>27</v>
+      </c>
       <c r="H3">
         <v>2</v>
       </c>

</xml_diff>